<commit_message>
All analysis and figure code is now working, just needs a bit more refactoring and documentation, and ideally setup with texlive.
</commit_message>
<xml_diff>
--- a/tables/regression_table.xlsx
+++ b/tables/regression_table.xlsx
@@ -473,37 +473,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.011*
+          <t>0.011
  (0.019)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.076*
+          <t>0.076
  (0.062)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.007*
+          <t>0.007
  (0.012)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.012*
+          <t>0.012
  (0.037)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-0.017**
+          <t>-0.017*
  (0.010)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-0.006*
+          <t>-0.006
  (0.026)</t>
         </is>
       </c>
@@ -516,7 +516,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-0.391****
+          <t>-0.391***
  (0.102)</t>
         </is>
       </c>
@@ -528,7 +528,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.516**********
+          <t>0.516***
  (0.067)</t>
         </is>
       </c>
@@ -540,13 +540,13 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.380**********
+          <t>0.380***
  (0.052)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.102*
+          <t>0.102
  (0.090)</t>
         </is>
       </c>
@@ -559,21 +559,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.291**
+          <t>0.291*
  (0.174)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.071*
+          <t>0.071
  (0.113)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.168**
+          <t>0.168*
  (0.094)</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Edits to some figures for readability; made another appendix figure.
</commit_message>
<xml_diff>
--- a/tables/regression_table.xlsx
+++ b/tables/regression_table.xlsx
@@ -473,38 +473,38 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.011
- (0.019)</t>
+          <t>0.006
+ (0.020)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.076
- (0.062)</t>
+          <t>0.043
+ (0.053)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.007
- (0.012)</t>
+          <t>0.010
+ (0.014)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.012
- (0.037)</t>
+          <t>0.002
+ (0.034)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-0.017*
- (0.010)</t>
+          <t>-0.010
+ (0.011)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-0.006
- (0.026)</t>
+          <t>0.013
+ (0.024)</t>
         </is>
       </c>
     </row>
@@ -516,38 +516,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-0.391***
- (0.102)</t>
+          <t>-0.366***
+ (0.115)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.538**
- (0.218)</t>
+          <t>-0.594**
+ (0.226)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.516***
- (0.067)</t>
+          <t>0.472***
+ (0.082)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.298**
- (0.130)</t>
+          <t>0.240
+ (0.147)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.380***
- (0.052)</t>
+          <t>0.341***
+ (0.062)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.102
- (0.090)</t>
+          <t>0.137
+ (0.100)</t>
         </is>
       </c>
     </row>
@@ -559,22 +559,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.291*
- (0.174)</t>
+          <t>0.311*
+ (0.181)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.071
- (0.113)</t>
+          <t>0.079
+ (0.126)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.168*
- (0.094)</t>
+          <t>0.138
+ (0.102)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -586,22 +586,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2891788384589128</v>
+        <v>0.2839416083222908</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1298369586866799</v>
+        <v>0.1533856611860601</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5715037721284368</v>
+        <v>0.4885907484925434</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1093231782710605</v>
+        <v>0.06683910056541831</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4639034034782142</v>
+        <v>0.3711881025611223</v>
       </c>
       <c r="G5" t="n">
-        <v>0.02501522138248546</v>
+        <v>0.04549049054619092</v>
       </c>
     </row>
     <row r="6">
@@ -611,22 +611,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C6" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E6" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F6" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G6" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Double-checked and altered a couple Misc. Energy classifications
</commit_message>
<xml_diff>
--- a/tables/regression_table.xlsx
+++ b/tables/regression_table.xlsx
@@ -479,13 +479,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.043
+          <t>0.044
  (0.053)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.010
+          <t>0.011
  (0.014)</t>
         </is>
       </c>
@@ -497,14 +497,14 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-0.010
+          <t>-0.011
  (0.011)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.013
- (0.024)</t>
+          <t>0.019
+ (0.023)</t>
         </is>
       </c>
     </row>
@@ -516,38 +516,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-0.366***
+          <t>-0.370***
  (0.115)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.594**
+          <t>-0.589**
  (0.226)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.472***
+          <t>0.468***
  (0.082)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.240
+          <t>0.236
  (0.147)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.341***
- (0.062)</t>
+          <t>0.343***
+ (0.061)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.137
- (0.100)</t>
+          <t>0.141
+ (0.099)</t>
         </is>
       </c>
     </row>
@@ -559,22 +559,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.311*
+          <t>0.308*
  (0.181)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.079
+          <t>0.071
  (0.126)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.138
- (0.102)</t>
+          <t>0.151
+ (0.100)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -586,22 +586,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2839416083222908</v>
+        <v>0.2857796200381378</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1533856611860601</v>
+        <v>0.1516449335735305</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4885907484925434</v>
+        <v>0.4886088471351145</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06683910056541831</v>
+        <v>0.06520864925664716</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3711881025611223</v>
+        <v>0.3805361884847204</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04549049054619092</v>
+        <v>0.0551647097794542</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
reran and fixed robustness check figure code
</commit_message>
<xml_diff>
--- a/tables/regression_table.xlsx
+++ b/tables/regression_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,199 +468,227 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Mining</t>
+          <t>Intercept</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.006
- (0.020)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.044
- (0.053)</t>
-        </is>
-      </c>
+          <t>0.244**
+ (0.096)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.011
- (0.014)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.002
- (0.034)</t>
-        </is>
-      </c>
+          <t>0.343***
+ (0.068)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-0.011
- (0.011)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.019
- (0.023)</t>
-        </is>
-      </c>
+          <t>0.511***
+ (0.052)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Partisanship</t>
+          <t>Mining</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-0.370***
- (0.115)</t>
+          <t>0.006
+ (0.020)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.589**
- (0.226)</t>
+          <t>0.044
+ (0.053)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.468***
- (0.082)</t>
+          <t>0.011
+ (0.014)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.236
- (0.147)</t>
+          <t>0.002
+ (0.034)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.343***
- (0.061)</t>
+          <t>-0.011
+ (0.011)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.141
- (0.099)</t>
+          <t>0.019
+ (0.023)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Deregulated</t>
+          <t>Partisanship</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.308*
- (0.181)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>-0.370***
+ (0.115)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-0.589**
+ (0.226)</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.071
- (0.126)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>0.468***
+ (0.082)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.236
+ (0.147)</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.151
- (0.100)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
+          <t>0.343***
+ (0.061)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.141
+ (0.099)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>R-squared</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.2857796200381378</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1516449335735305</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.4886088471351145</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.06520864925664716</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3805361884847204</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0551647097794542</v>
-      </c>
+          <t>Deregulated</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.308*
+ (0.181)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.071
+ (0.126)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.151
+ (0.100)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>R-squared</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>56</v>
+        <v>0.2857796200381378</v>
       </c>
       <c r="C6" t="n">
-        <v>56</v>
+        <v>0.1516449335735305</v>
       </c>
       <c r="D6" t="n">
-        <v>49</v>
+        <v>0.4886088471351145</v>
       </c>
       <c r="E6" t="n">
-        <v>49</v>
+        <v>0.06520864925664716</v>
       </c>
       <c r="F6" t="n">
-        <v>57</v>
+        <v>0.3805361884847204</v>
       </c>
       <c r="G6" t="n">
-        <v>57</v>
+        <v>0.0551647097794542</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>56</v>
+      </c>
+      <c r="C7" t="n">
+        <v>56</v>
+      </c>
+      <c r="D7" t="n">
+        <v>49</v>
+      </c>
+      <c r="E7" t="n">
+        <v>49</v>
+      </c>
+      <c r="F7" t="n">
+        <v>57</v>
+      </c>
+      <c r="G7" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
           <t>State FE</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>

<commit_message>
Fixed year indexing in structural_factors.py
</commit_message>
<xml_diff>
--- a/tables/regression_table.xlsx
+++ b/tables/regression_table.xlsx
@@ -473,22 +473,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.244**
- (0.096)</t>
+          <t>0.237***
+ (0.087)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.343***
- (0.068)</t>
+          <t>0.355***
+ (0.060)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.511***
- (0.052)</t>
+          <t>0.521***
+ (0.047)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -501,37 +501,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.006
- (0.020)</t>
+          <t>0.010
+ (0.019)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.044
- (0.053)</t>
+          <t>0.049
+ (0.055)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.011
- (0.014)</t>
+          <t>0.008
+ (0.012)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.002
+          <t>0.005
  (0.034)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-0.011
- (0.011)</t>
+          <t>-0.017
+ (0.010)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.019
+          <t>0.003
  (0.023)</t>
         </is>
       </c>
@@ -544,38 +544,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-0.370***
- (0.115)</t>
+          <t>-0.385***
+ (0.099)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.589**
- (0.226)</t>
+          <t>-0.545**
+ (0.214)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.468***
- (0.082)</t>
+          <t>0.504***
+ (0.067)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.236
- (0.147)</t>
+          <t>0.294**
+ (0.134)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.343***
- (0.061)</t>
+          <t>0.376***
+ (0.052)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.141
- (0.099)</t>
+          <t>0.109
+ (0.091)</t>
         </is>
       </c>
     </row>
@@ -587,22 +587,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.308*
- (0.181)</t>
+          <t>0.291*
+ (0.169)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.071
- (0.126)</t>
+          <t>0.078
+ (0.113)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.151
- (0.100)</t>
+          <t>0.179*
+ (0.093)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -614,22 +614,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2857796200381378</v>
+        <v>0.2962603545018835</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1516449335735305</v>
+        <v>0.130089143551553</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4886088471351145</v>
+        <v>0.5616280652897079</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06520864925664716</v>
+        <v>0.1011422130944299</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3805361884847204</v>
+        <v>0.4634153834670367</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0551647097794542</v>
+        <v>0.02731738325835731</v>
       </c>
     </row>
     <row r="7">
@@ -639,22 +639,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C7" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E7" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F7" t="n">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G7" t="n">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">

</xml_diff>